<commit_message>
Update scraping part. New datas are appending
</commit_message>
<xml_diff>
--- a/Data Files/bitcoin/xlsx Files/prices.xlsx
+++ b/Data Files/bitcoin/xlsx Files/prices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="1310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="1321">
   <si>
     <t>date</t>
   </si>
@@ -3944,6 +3944,39 @@
   </si>
   <si>
     <t>2023-07-31</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>2023-08-02</t>
+  </si>
+  <si>
+    <t>2023-08-03</t>
+  </si>
+  <si>
+    <t>2023-08-04</t>
+  </si>
+  <si>
+    <t>2023-08-05</t>
+  </si>
+  <si>
+    <t>2023-08-06</t>
+  </si>
+  <si>
+    <t>2023-08-07</t>
+  </si>
+  <si>
+    <t>2023-08-08</t>
+  </si>
+  <si>
+    <t>2023-08-09</t>
+  </si>
+  <si>
+    <t>2023-08-10</t>
+  </si>
+  <si>
+    <t>2023-08-11</t>
   </si>
 </sst>
 </file>
@@ -4301,7 +4334,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1309"/>
+  <dimension ref="A1:B1320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4616,7 +4649,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>9744.636578159387</v>
+        <v>9744.636578159389</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4744,7 +4777,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>9658.606058375473</v>
+        <v>9658.606058375472</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5440,7 +5473,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>9760.198937162193</v>
+        <v>9760.198937162191</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -5456,7 +5489,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>9059.962506871727</v>
+        <v>9059.962506871729</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -5464,7 +5497,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>9131.767275081993</v>
+        <v>9131.767275081991</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -5472,7 +5505,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>9170.361063506127</v>
+        <v>9170.361063506129</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -5576,7 +5609,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>9636.965527050057</v>
+        <v>9636.965527050055</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -5584,7 +5617,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>9662.858709002241</v>
+        <v>9662.858709002239</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -5592,7 +5625,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>9738.603356828593</v>
+        <v>9738.603356828591</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -5648,7 +5681,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>9345.960907722063</v>
+        <v>9345.960907722065</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -5672,7 +5705,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>9463.361414311787</v>
+        <v>9463.361414311788</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -5792,7 +5825,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>9094.318072166905</v>
+        <v>9094.318072166903</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -5832,7 +5865,7 @@
         <v>191</v>
       </c>
       <c r="B191">
-        <v>9253.630980242333</v>
+        <v>9253.630980242331</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -5840,7 +5873,7 @@
         <v>192</v>
       </c>
       <c r="B192">
-        <v>9432.172515827939</v>
+        <v>9432.172515827941</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -5864,7 +5897,7 @@
         <v>195</v>
       </c>
       <c r="B195">
-        <v>9234.314674712627</v>
+        <v>9234.314674712628</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -5888,7 +5921,7 @@
         <v>198</v>
       </c>
       <c r="B198">
-        <v>9247.060695963813</v>
+        <v>9247.060695963812</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -5896,7 +5929,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>9203.371435179699</v>
+        <v>9203.371435179701</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -5944,7 +5977,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>9384.379751903267</v>
+        <v>9384.379751903269</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -5992,7 +6025,7 @@
         <v>211</v>
       </c>
       <c r="B211">
-        <v>10962.25848120735</v>
+        <v>10962.25848120736</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -6016,7 +6049,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>11116.30716368527</v>
+        <v>11116.30716368528</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -6032,7 +6065,7 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>11812.09430726851</v>
+        <v>11812.09430726852</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -6056,7 +6089,7 @@
         <v>219</v>
       </c>
       <c r="B219">
-        <v>11181.91750803489</v>
+        <v>11181.91750803488</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -6120,7 +6153,7 @@
         <v>227</v>
       </c>
       <c r="B227">
-        <v>11579.86795160213</v>
+        <v>11579.86795160214</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -6416,7 +6449,7 @@
         <v>264</v>
       </c>
       <c r="B264">
-        <v>10927.15031029327</v>
+        <v>10927.15031029328</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -6512,7 +6545,7 @@
         <v>276</v>
       </c>
       <c r="B276">
-        <v>10770.88134746641</v>
+        <v>10770.88134746642</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -7168,7 +7201,7 @@
         <v>358</v>
       </c>
       <c r="B358">
-        <v>22840.99170718835</v>
+        <v>22840.99170718836</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -7200,7 +7233,7 @@
         <v>362</v>
       </c>
       <c r="B362">
-        <v>24671.10771441542</v>
+        <v>24671.10771441541</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -7896,7 +7929,7 @@
         <v>449</v>
       </c>
       <c r="B449">
-        <v>54370.13755789518</v>
+        <v>54370.13755789519</v>
       </c>
     </row>
     <row r="450" spans="1:2">
@@ -8040,7 +8073,7 @@
         <v>467</v>
       </c>
       <c r="B467">
-        <v>58152.99326214183</v>
+        <v>58152.99326214184</v>
       </c>
     </row>
     <row r="468" spans="1:2">
@@ -8072,7 +8105,7 @@
         <v>471</v>
       </c>
       <c r="B471">
-        <v>63576.67604104827</v>
+        <v>63576.67604104828</v>
       </c>
     </row>
     <row r="472" spans="1:2">
@@ -8096,7 +8129,7 @@
         <v>474</v>
       </c>
       <c r="B474">
-        <v>61497.29956944119</v>
+        <v>61497.2995694412</v>
       </c>
     </row>
     <row r="475" spans="1:2">
@@ -8256,7 +8289,7 @@
         <v>494</v>
       </c>
       <c r="B494">
-        <v>56507.75943986959</v>
+        <v>56507.7594398696</v>
       </c>
     </row>
     <row r="495" spans="1:2">
@@ -8312,7 +8345,7 @@
         <v>501</v>
       </c>
       <c r="B501">
-        <v>49972.79539837244</v>
+        <v>49972.79539837245</v>
       </c>
     </row>
     <row r="502" spans="1:2">
@@ -8480,7 +8513,7 @@
         <v>522</v>
       </c>
       <c r="B522">
-        <v>39151.31618380031</v>
+        <v>39151.31618380032</v>
       </c>
     </row>
     <row r="523" spans="1:2">
@@ -8592,7 +8625,7 @@
         <v>536</v>
       </c>
       <c r="B536">
-        <v>38193.61914194396</v>
+        <v>38193.61914194397</v>
       </c>
     </row>
     <row r="537" spans="1:2">
@@ -9008,7 +9041,7 @@
         <v>588</v>
       </c>
       <c r="B588">
-        <v>43753.21786264631</v>
+        <v>43753.21786264632</v>
       </c>
     </row>
     <row r="589" spans="1:2">
@@ -9080,7 +9113,7 @@
         <v>597</v>
       </c>
       <c r="B597">
-        <v>44534.4548542199</v>
+        <v>44534.45485421991</v>
       </c>
     </row>
     <row r="598" spans="1:2">
@@ -9168,7 +9201,7 @@
         <v>608</v>
       </c>
       <c r="B608">
-        <v>48936.5372541422</v>
+        <v>48936.53725414221</v>
       </c>
     </row>
     <row r="609" spans="1:2">
@@ -9240,7 +9273,7 @@
         <v>617</v>
       </c>
       <c r="B617">
-        <v>52739.80016634551</v>
+        <v>52739.80016634552</v>
       </c>
     </row>
     <row r="618" spans="1:2">
@@ -9392,7 +9425,7 @@
         <v>636</v>
       </c>
       <c r="B636">
-        <v>42856.85516422451</v>
+        <v>42856.85516422452</v>
       </c>
     </row>
     <row r="637" spans="1:2">
@@ -9408,7 +9441,7 @@
         <v>638</v>
       </c>
       <c r="B638">
-        <v>42247.35572900635</v>
+        <v>42247.35572900636</v>
       </c>
     </row>
     <row r="639" spans="1:2">
@@ -9504,7 +9537,7 @@
         <v>650</v>
       </c>
       <c r="B650">
-        <v>55125.46033768044</v>
+        <v>55125.46033768045</v>
       </c>
     </row>
     <row r="651" spans="1:2">
@@ -9536,7 +9569,7 @@
         <v>654</v>
       </c>
       <c r="B654">
-        <v>57487.98588042219</v>
+        <v>57487.9858804222</v>
       </c>
     </row>
     <row r="655" spans="1:2">
@@ -9800,7 +9833,7 @@
         <v>687</v>
       </c>
       <c r="B687">
-        <v>63933.83544259932</v>
+        <v>63933.83544259933</v>
       </c>
     </row>
     <row r="688" spans="1:2">
@@ -10256,7 +10289,7 @@
         <v>744</v>
       </c>
       <c r="B744">
-        <v>42777.21102048235</v>
+        <v>42777.21102048236</v>
       </c>
     </row>
     <row r="745" spans="1:2">
@@ -10584,7 +10617,7 @@
         <v>785</v>
       </c>
       <c r="B785">
-        <v>37059.97940228751</v>
+        <v>37059.97940228752</v>
       </c>
     </row>
     <row r="786" spans="1:2">
@@ -10816,7 +10849,7 @@
         <v>814</v>
       </c>
       <c r="B814">
-        <v>42401.89559748943</v>
+        <v>42401.89559748944</v>
       </c>
     </row>
     <row r="815" spans="1:2">
@@ -10976,7 +11009,7 @@
         <v>834</v>
       </c>
       <c r="B834">
-        <v>39603.96515928415</v>
+        <v>39603.96515928416</v>
       </c>
     </row>
     <row r="835" spans="1:2">
@@ -11288,7 +11321,7 @@
         <v>873</v>
       </c>
       <c r="B873">
-        <v>29256.81337441626</v>
+        <v>29256.81337441625</v>
       </c>
     </row>
     <row r="874" spans="1:2">
@@ -11440,7 +11473,7 @@
         <v>892</v>
       </c>
       <c r="B892">
-        <v>30229.23683613038</v>
+        <v>30229.23683613037</v>
       </c>
     </row>
     <row r="893" spans="1:2">
@@ -11472,7 +11505,7 @@
         <v>896</v>
       </c>
       <c r="B896">
-        <v>26767.26917322131</v>
+        <v>26767.26917322132</v>
       </c>
     </row>
     <row r="897" spans="1:2">
@@ -11624,7 +11657,7 @@
         <v>915</v>
       </c>
       <c r="B915">
-        <v>19407.44743026247</v>
+        <v>19407.44743026248</v>
       </c>
     </row>
     <row r="916" spans="1:2">
@@ -11640,7 +11673,7 @@
         <v>917</v>
       </c>
       <c r="B917">
-        <v>19310.23321852183</v>
+        <v>19310.23321852184</v>
       </c>
     </row>
     <row r="918" spans="1:2">
@@ -11800,7 +11833,7 @@
         <v>937</v>
       </c>
       <c r="B937">
-        <v>22506.19957362899</v>
+        <v>22506.19957362898</v>
       </c>
     </row>
     <row r="938" spans="1:2">
@@ -11824,7 +11857,7 @@
         <v>940</v>
       </c>
       <c r="B940">
-        <v>21235.61231608578</v>
+        <v>21235.61231608577</v>
       </c>
     </row>
     <row r="941" spans="1:2">
@@ -11944,7 +11977,7 @@
         <v>955</v>
       </c>
       <c r="B955">
-        <v>23948.82955327163</v>
+        <v>23948.82955327164</v>
       </c>
     </row>
     <row r="956" spans="1:2">
@@ -12288,7 +12321,7 @@
         <v>998</v>
       </c>
       <c r="B998">
-        <v>19464.32266334847</v>
+        <v>19464.32266334846</v>
       </c>
     </row>
     <row r="999" spans="1:2">
@@ -12336,7 +12369,7 @@
         <v>1004</v>
       </c>
       <c r="B1004">
-        <v>19444.78777136298</v>
+        <v>19444.78777136297</v>
       </c>
     </row>
     <row r="1005" spans="1:2">
@@ -12432,7 +12465,7 @@
         <v>1016</v>
       </c>
       <c r="B1016">
-        <v>19142.6947673929</v>
+        <v>19142.69476739289</v>
       </c>
     </row>
     <row r="1017" spans="1:2">
@@ -12448,7 +12481,7 @@
         <v>1018</v>
       </c>
       <c r="B1018">
-        <v>19153.03977998699</v>
+        <v>19153.03977998698</v>
       </c>
     </row>
     <row r="1019" spans="1:2">
@@ -12560,7 +12593,7 @@
         <v>1032</v>
       </c>
       <c r="B1032">
-        <v>20774.24749642603</v>
+        <v>20774.24749642604</v>
       </c>
     </row>
     <row r="1033" spans="1:2">
@@ -12656,7 +12689,7 @@
         <v>1044</v>
       </c>
       <c r="B1044">
-        <v>20597.75501706083</v>
+        <v>20597.75501706084</v>
       </c>
     </row>
     <row r="1045" spans="1:2">
@@ -13360,7 +13393,7 @@
         <v>1132</v>
       </c>
       <c r="B1132">
-        <v>23451.57765077463</v>
+        <v>23451.57765077464</v>
       </c>
     </row>
     <row r="1133" spans="1:2">
@@ -13376,7 +13409,7 @@
         <v>1134</v>
       </c>
       <c r="B1134">
-        <v>22946.28657859123</v>
+        <v>22946.28657859124</v>
       </c>
     </row>
     <row r="1135" spans="1:2">
@@ -13408,7 +13441,7 @@
         <v>1138</v>
       </c>
       <c r="B1138">
-        <v>21820.88650809278</v>
+        <v>21820.88650809277</v>
       </c>
     </row>
     <row r="1139" spans="1:2">
@@ -13512,7 +13545,7 @@
         <v>1151</v>
       </c>
       <c r="B1151">
-        <v>24146.10136454522</v>
+        <v>24146.10136454523</v>
       </c>
     </row>
     <row r="1152" spans="1:2">
@@ -13568,7 +13601,7 @@
         <v>1158</v>
       </c>
       <c r="B1158">
-        <v>23634.33348912379</v>
+        <v>23634.33348912378</v>
       </c>
     </row>
     <row r="1159" spans="1:2">
@@ -13760,7 +13793,7 @@
         <v>1182</v>
       </c>
       <c r="B1182">
-        <v>27670.19949849683</v>
+        <v>27670.19949849684</v>
       </c>
     </row>
     <row r="1183" spans="1:2">
@@ -14040,7 +14073,7 @@
         <v>1217</v>
       </c>
       <c r="B1217">
-        <v>29217.94404680991</v>
+        <v>29217.94404680992</v>
       </c>
     </row>
     <row r="1218" spans="1:2">
@@ -14048,7 +14081,7 @@
         <v>1218</v>
       </c>
       <c r="B1218">
-        <v>29362.05621362539</v>
+        <v>29362.0562136254</v>
       </c>
     </row>
     <row r="1219" spans="1:2">
@@ -14072,7 +14105,7 @@
         <v>1221</v>
       </c>
       <c r="B1221">
-        <v>28988.32099624927</v>
+        <v>28988.32099624928</v>
       </c>
     </row>
     <row r="1222" spans="1:2">
@@ -14224,7 +14257,7 @@
         <v>1240</v>
       </c>
       <c r="B1240">
-        <v>26869.68602179078</v>
+        <v>26869.68602179077</v>
       </c>
     </row>
     <row r="1241" spans="1:2">
@@ -14248,7 +14281,7 @@
         <v>1243</v>
       </c>
       <c r="B1243">
-        <v>26475.60790253427</v>
+        <v>26475.60790253428</v>
       </c>
     </row>
     <row r="1244" spans="1:2">
@@ -14352,7 +14385,7 @@
         <v>1256</v>
       </c>
       <c r="B1256">
-        <v>26346.24454513763</v>
+        <v>26346.24454513764</v>
       </c>
     </row>
     <row r="1257" spans="1:2">
@@ -14432,7 +14465,7 @@
         <v>1266</v>
       </c>
       <c r="B1266">
-        <v>26501.04444223367</v>
+        <v>26501.04444223368</v>
       </c>
     </row>
     <row r="1267" spans="1:2">
@@ -14488,7 +14521,7 @@
         <v>1273</v>
       </c>
       <c r="B1273">
-        <v>30537.81666463479</v>
+        <v>30537.8166646348</v>
       </c>
     </row>
     <row r="1274" spans="1:2">
@@ -14752,7 +14785,7 @@
         <v>1306</v>
       </c>
       <c r="B1306">
-        <v>29200.24400129131</v>
+        <v>29200.24400129132</v>
       </c>
     </row>
     <row r="1307" spans="1:2">
@@ -14777,6 +14810,94 @@
       </c>
       <c r="B1309">
         <v>29277.75581027272</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:2">
+      <c r="A1310" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B1310">
+        <v>29257.22551026271</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:2">
+      <c r="A1311" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B1311">
+        <v>29163.6056046116</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:2">
+      <c r="A1312" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B1312">
+        <v>29258.09780169691</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:2">
+      <c r="A1313" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B1313">
+        <v>28994.49595265385</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:2">
+      <c r="A1314" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B1314">
+        <v>29036.34608849958</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:2">
+      <c r="A1315" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B1315">
+        <v>29044.47746048231</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:2">
+      <c r="A1316" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B1316">
+        <v>29070.22569492281</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:2">
+      <c r="A1317" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B1317">
+        <v>29842.8071494232</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:2">
+      <c r="A1318" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B1318">
+        <v>29482.86136198899</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:2">
+      <c r="A1319" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B1319">
+        <v>29406.76406270633</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:2">
+      <c r="A1320" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B1320">
+        <v>29361.80661261011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>